<commit_message>
Testing bam_file entry counter
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7180" yWindow="0" windowWidth="21540" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Entry number</t>
   </si>
@@ -122,50 +122,68 @@
     <t>C1</t>
   </si>
   <si>
+    <t>BAM2</t>
+  </si>
+  <si>
+    <t>pub2</t>
+  </si>
+  <si>
+    <t>NCBI2</t>
+  </si>
+  <si>
+    <t>sub2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>title2</t>
+  </si>
+  <si>
+    <t>Please fill in the Data Sheet with your RNA-Seq experiment information. For the list of plant tissue file names, please refer to the SVG directory tab.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>E-MTAB-1668:24hCS-RNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique descriptor of experiment </t>
+  </si>
+  <si>
+    <t>Desc1</t>
+  </si>
+  <si>
+    <t>test2.svg</t>
+  </si>
+  <si>
+    <t>Desc 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
     <t>R1, R2</t>
   </si>
   <si>
-    <t>BAM2</t>
-  </si>
-  <si>
-    <t>pub2</t>
-  </si>
-  <si>
-    <t>NCBI2</t>
-  </si>
-  <si>
-    <t>sub2</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
-    <t>title2</t>
-  </si>
-  <si>
-    <t>species2</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
-  <si>
-    <t>asdas</t>
-  </si>
-  <si>
-    <t>Please fill in the Data Sheet with your RNA-Seq experiment information. For the list of plant tissue file names, please refer to the SVG directory tab.</t>
+    <t>A. thaliana</t>
+  </si>
+  <si>
+    <t>Germinating seeds 2</t>
+  </si>
+  <si>
+    <t>amazons3.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,6 +240,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +320,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -308,6 +331,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -324,7 +348,24 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -661,6 +702,23 @@
           <bgColor theme="6"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -887,49 +945,51 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <oleLink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" progId="Word.Document.12">
     <oleItems>
-      <oleItem name="'" icon="1" preferPic="1"/>
+      <oleItem name="'" preferPic="1"/>
     </oleItems>
   </oleLink>
 </externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K3" totalsRowShown="0">
-  <autoFilter ref="A1:K3"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L3" totalsRowShown="0">
+  <autoFilter ref="A1:L3"/>
+  <tableColumns count="12">
     <tableColumn id="1" name="Entry number">
       <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Species" dataDxfId="24"/>
-    <tableColumn id="11" name="Title" dataDxfId="23"/>
-    <tableColumn id="2" name="BAM link" dataDxfId="22"/>
-    <tableColumn id="3" name="Publication URL" dataDxfId="21"/>
-    <tableColumn id="4" name="NCBI link" dataDxfId="20"/>
-    <tableColumn id="5" name="Total reads mapped " dataDxfId="19"/>
-    <tableColumn id="9" name="Tissue" dataDxfId="18"/>
-    <tableColumn id="6" name="Tissue subunit " dataDxfId="17"/>
-    <tableColumn id="7" name="Controls" dataDxfId="16"/>
-    <tableColumn id="8" name="Replicates" dataDxfId="15"/>
+    <tableColumn id="10" name="Species" dataDxfId="26"/>
+    <tableColumn id="11" name="Title" dataDxfId="25"/>
+    <tableColumn id="2" name="BAM link" dataDxfId="24"/>
+    <tableColumn id="3" name="Publication URL" dataDxfId="23"/>
+    <tableColumn id="4" name="NCBI link" dataDxfId="22"/>
+    <tableColumn id="5" name="Total reads mapped " dataDxfId="21"/>
+    <tableColumn id="9" name="Tissue" dataDxfId="20"/>
+    <tableColumn id="6" name="Tissue subunit " dataDxfId="19"/>
+    <tableColumn id="7" name="Controls" dataDxfId="18"/>
+    <tableColumn id="8" name="Replicates" dataDxfId="17"/>
+    <tableColumn id="12" name="Description " dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:L6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" tableBorderDxfId="11">
-  <autoFilter ref="B4:L6"/>
-  <tableColumns count="11">
-    <tableColumn id="1" name="Entry number" dataDxfId="10"/>
-    <tableColumn id="2" name="Species" dataDxfId="9"/>
-    <tableColumn id="3" name="Title" dataDxfId="8"/>
-    <tableColumn id="4" name="BAM link" dataDxfId="7"/>
-    <tableColumn id="5" name="Publication URL" dataDxfId="6"/>
-    <tableColumn id="6" name="NCBI link" dataDxfId="5"/>
-    <tableColumn id="7" name="Total reads mapped " dataDxfId="4"/>
-    <tableColumn id="8" name="Tissue" dataDxfId="3"/>
-    <tableColumn id="9" name="Tissue subunit " dataDxfId="2"/>
-    <tableColumn id="10" name="Controls" dataDxfId="1"/>
-    <tableColumn id="11" name="Replicates" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B4:M6" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12">
+  <autoFilter ref="B4:M6"/>
+  <tableColumns count="12">
+    <tableColumn id="1" name="Entry number" dataDxfId="11"/>
+    <tableColumn id="2" name="Species" dataDxfId="10"/>
+    <tableColumn id="3" name="Title" dataDxfId="9"/>
+    <tableColumn id="4" name="BAM link" dataDxfId="8"/>
+    <tableColumn id="5" name="Publication URL" dataDxfId="7"/>
+    <tableColumn id="6" name="NCBI link" dataDxfId="6"/>
+    <tableColumn id="7" name="Total reads mapped " dataDxfId="5"/>
+    <tableColumn id="8" name="Tissue" dataDxfId="4"/>
+    <tableColumn id="9" name="Tissue subunit " dataDxfId="3"/>
+    <tableColumn id="10" name="Controls" dataDxfId="2"/>
+    <tableColumn id="11" name="Replicates" dataDxfId="1"/>
+    <tableColumn id="12" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1257,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1278,7 +1338,7 @@
     <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1312,18 +1372,23 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2">
         <f>ROW(A1)</f>
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>27</v>
@@ -1331,9 +1396,7 @@
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="9">
-        <v>1000</v>
-      </c>
+      <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
         <v>29</v>
       </c>
@@ -1344,43 +1407,49 @@
         <v>31</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3">
         <f t="shared" ref="A3" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>35</v>
       </c>
       <c r="G3" s="9">
         <v>2000</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I3" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>38</v>
+      <c r="L3" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1399,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1418,24 +1487,25 @@
     <col min="10" max="10" width="18.5" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="48" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:13">
       <c r="A3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1469,8 +1539,11 @@
       <c r="L4" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="M4" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" ht="16">
+    <row r="5" spans="1:13" ht="17">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -1504,8 +1577,11 @@
       <c r="L5" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="M5" s="10" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" ht="16">
+    <row r="6" spans="1:13" ht="16">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1524,10 +1600,13 @@
       <c r="L6" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="M6" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submission UI change and excel parser
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="0" windowWidth="21540" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
   <si>
     <t>Entry number</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>amazons3.com</t>
+  </si>
+  <si>
+    <t>R2, R3, r4, r5</t>
   </si>
 </sst>
 </file>
@@ -267,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -304,8 +307,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -319,8 +344,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,20 +359,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
@@ -952,8 +984,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L3" totalsRowShown="0">
-  <autoFilter ref="A1:L3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L4" totalsRowShown="0">
+  <autoFilter ref="A1:L4"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Entry number">
       <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
@@ -1317,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1396,7 +1428,9 @@
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="9">
+        <v>2433</v>
+      </c>
       <c r="H2" s="9" t="s">
         <v>29</v>
       </c>
@@ -1415,7 +1449,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3">
-        <f t="shared" ref="A3" si="0">ROW(A2)</f>
+        <f t="shared" ref="A3:A4" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1449,6 +1483,45 @@
         <v>37</v>
       </c>
       <c r="L3" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="12">
+        <v>2000</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="13" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change submissions system aesthetics
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>Entry number</t>
   </si>
@@ -107,42 +107,6 @@
     <t xml:space="preserve">Note: file and subunit names are case and punctuation sensitive, so please copy and paste into the data sheet. </t>
   </si>
   <si>
-    <t>Pub1</t>
-  </si>
-  <si>
-    <t>NCBI1</t>
-  </si>
-  <si>
-    <t>test.svg</t>
-  </si>
-  <si>
-    <t>sub1</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>BAM2</t>
-  </si>
-  <si>
-    <t>pub2</t>
-  </si>
-  <si>
-    <t>NCBI2</t>
-  </si>
-  <si>
-    <t>sub2</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
-    <t>title2</t>
-  </si>
-  <si>
     <t>Please fill in the Data Sheet with your RNA-Seq experiment information. For the list of plant tissue file names, please refer to the SVG directory tab.</t>
   </si>
   <si>
@@ -155,38 +119,53 @@
     <t xml:space="preserve">Unique descriptor of experiment </t>
   </si>
   <si>
-    <t>Desc1</t>
-  </si>
-  <si>
-    <t>test2.svg</t>
-  </si>
-  <si>
-    <t>Desc 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description </t>
   </si>
   <si>
-    <t>R1, R2</t>
-  </si>
-  <si>
     <t>A. thaliana</t>
   </si>
   <si>
-    <t>Germinating seeds 2</t>
-  </si>
-  <si>
-    <t>amazons3.com</t>
-  </si>
-  <si>
-    <t>R2, R3, r4, r5</t>
+    <t>Internode.svg</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>LeafParts.svg</t>
+  </si>
+  <si>
+    <t>lamina</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/iplant-cdn/iplant/home/araport/rnaseq_bam/aerial/SRR547531/accepted_hits.bam</t>
+  </si>
+  <si>
+    <t>Transcription profiling of Arabidopsis plants overexpressing SlHsfA3 (thale cress)</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/23349984</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/Traces/sra/?run=SRR547531</t>
+  </si>
+  <si>
+    <t>SRR547531</t>
+  </si>
+  <si>
+    <t>SRR547531, SRR547532, SRR547533</t>
+  </si>
+  <si>
+    <t>GSM798296: mRNASeq_WT_rep2</t>
+  </si>
+  <si>
+    <t>If you want to clear contents of an entry, be sure to click 'Delete Entire Row' to prevent errors. Thanks!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -249,6 +228,12 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -270,7 +255,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -307,30 +292,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="6" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -346,8 +309,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -359,11 +324,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -371,6 +335,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -378,6 +343,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
@@ -984,8 +950,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L4" totalsRowShown="0">
-  <autoFilter ref="A1:L4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L3" totalsRowShown="0">
+  <autoFilter ref="A1:L3"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Entry number">
       <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
@@ -1349,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1361,7 +1327,7 @@
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="20.83203125" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
@@ -1405,7 +1371,7 @@
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1414,118 +1380,80 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G2" s="9">
-        <v>2433</v>
+        <v>29098868</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3">
-        <f t="shared" ref="A3:A4" si="0">ROW(A2)</f>
+      <c r="A3" s="11">
+        <f t="shared" ref="A3" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="9">
-        <v>2000</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="D3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="12">
+        <v>13627154</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="11">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="12">
-        <v>2000</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>45</v>
+      <c r="J3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="1">
@@ -1541,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1613,7 +1541,7 @@
         <v>6</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="17">
@@ -1651,7 +1579,7 @@
         <v>20</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16">
@@ -1674,12 +1602,17 @@
         <v>23</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel conversion functional and modal changes
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="16056" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1824" windowWidth="25596" windowHeight="16056" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="FILL Basic" sheetId="5" r:id="rId1"/>
-    <sheet name="FILL Data" sheetId="1" r:id="rId2"/>
+    <sheet name="FILL Data" sheetId="1" r:id="rId1"/>
+    <sheet name="FILL Basic" sheetId="5" r:id="rId2"/>
     <sheet name="README" sheetId="3" r:id="rId3"/>
     <sheet name="SVG directory" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>Entry number</t>
   </si>
@@ -171,13 +171,55 @@
   </si>
   <si>
     <t>Anything marked with a * is considered required information and must be filled out</t>
+  </si>
+  <si>
+    <t>Replicate Control7</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Transcription profiling of Arabidopsis plants overexpressing SlHsfA3 (thale cress)</t>
+  </si>
+  <si>
+    <t>GSM798296: mRNASeq_WT_rep2</t>
+  </si>
+  <si>
+    <t>SRR547531</t>
+  </si>
+  <si>
+    <t>Rosette_Plus_Root</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/iplant-cdn/iplant/home/araport/rnaseq_bam/aerial/SRR547531/accepted_hits.bam</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/pubmed/23349984</t>
+  </si>
+  <si>
+    <t>http://www.ncbi.nlm.nih.gov/Traces/sra/?run=SRR547531</t>
+  </si>
+  <si>
+    <t>SRR547532</t>
+  </si>
+  <si>
+    <t>SRR547533</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,12 +294,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -364,7 +400,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -378,7 +414,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -407,42 +442,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -576,6 +575,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -644,6 +644,41 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -753,7 +788,7 @@
                   <a14:compatExt spid="_x0000_s4155"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00003B100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00003B100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -807,20 +842,20 @@
     <tableColumn id="11" name="Description*" dataDxfId="16"/>
     <tableColumn id="2" name="Record Number *" dataDxfId="15"/>
     <tableColumn id="3" name="RNA-Seq Data/BAM file repository link*" dataDxfId="14"/>
-    <tableColumn id="19" name="Repository type* (Amazon AWS or Google Drive)" dataDxfId="1"/>
-    <tableColumn id="4" name="Publication Link" dataDxfId="13"/>
-    <tableColumn id="5" name="SRA/NCBI Link" dataDxfId="12"/>
-    <tableColumn id="9" name="Total Reads Mapped*" dataDxfId="11"/>
-    <tableColumn id="6" name="Species*" dataDxfId="10"/>
-    <tableColumn id="7" name="Tissue*" dataDxfId="9"/>
-    <tableColumn id="20" name="Tissue subunit*" dataDxfId="0"/>
-    <tableColumn id="8" name="Controls" dataDxfId="8"/>
-    <tableColumn id="12" name="Replicate Control" dataDxfId="7"/>
-    <tableColumn id="13" name="Replicate Control2" dataDxfId="6"/>
-    <tableColumn id="14" name="Replicate Control3" dataDxfId="5"/>
-    <tableColumn id="15" name="Replicate Control4" dataDxfId="4"/>
-    <tableColumn id="16" name="Replicate Control5" dataDxfId="3"/>
-    <tableColumn id="17" name="Replicate Control6" dataDxfId="2"/>
+    <tableColumn id="19" name="Repository type* (Amazon AWS or Google Drive)" dataDxfId="13"/>
+    <tableColumn id="4" name="Publication Link" dataDxfId="12"/>
+    <tableColumn id="5" name="SRA/NCBI Link" dataDxfId="11"/>
+    <tableColumn id="9" name="Total Reads Mapped*" dataDxfId="10"/>
+    <tableColumn id="6" name="Species*" dataDxfId="9"/>
+    <tableColumn id="7" name="Tissue*" dataDxfId="8"/>
+    <tableColumn id="20" name="Tissue subunit*" dataDxfId="7"/>
+    <tableColumn id="8" name="Controls" dataDxfId="6"/>
+    <tableColumn id="12" name="Replicate Control" dataDxfId="5"/>
+    <tableColumn id="13" name="Replicate Control2" dataDxfId="4"/>
+    <tableColumn id="14" name="Replicate Control3" dataDxfId="3"/>
+    <tableColumn id="15" name="Replicate Control4" dataDxfId="2"/>
+    <tableColumn id="16" name="Replicate Control5" dataDxfId="1"/>
+    <tableColumn id="17" name="Replicate Control6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1148,75 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="15.296875" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.296875" customWidth="1"/>
-    <col min="6" max="8" width="20.796875" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="11.296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1301,48 +1271,112 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="B2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="10">
+        <v>29098868</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="10">
+        <v>13627154</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -1359,12 +1393,77 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="15.296875" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="17.296875" customWidth="1"/>
+    <col min="6" max="8" width="20.796875" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="10.796875" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="12" max="12" width="11.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1405,7 +1504,7 @@
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
@@ -1415,17 +1514,17 @@
       <c r="D4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-    </row>
-    <row r="5" spans="1:20" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
@@ -1435,31 +1534,31 @@
       <c r="D5" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="18"/>
-    </row>
-    <row r="6" spans="1:20" s="14" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="16"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1617,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Excel conversion and generating data bug fixes
Fixed order of data in Excel version in XMLgenerator-v2, fixed the
submit button in generating new data in Submission_page. as well as
aesthetic modal changes in index.html
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1824" windowWidth="25596" windowHeight="16056" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2430" windowWidth="25590" windowHeight="16050" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="FILL Data" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>Entry number</t>
   </si>
@@ -173,21 +173,6 @@
     <t>Anything marked with a * is considered required information and must be filled out</t>
   </si>
   <si>
-    <t>Replicate Control7</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Transcription profiling of Arabidopsis plants overexpressing SlHsfA3 (thale cress)</t>
   </si>
   <si>
@@ -213,13 +198,37 @@
   </si>
   <si>
     <t>SRR547533</t>
+  </si>
+  <si>
+    <t>Arabidopsis thaliana Flowers 12-14</t>
+  </si>
+  <si>
+    <t>1 ILLUMINA (Illumina HiSeq 2000) run: 25.1M spots, 1.3G bases, 806.8Mb downloads</t>
+  </si>
+  <si>
+    <t>SRR3581866</t>
+  </si>
+  <si>
+    <t>http://bar.utoronto.ca/~asullivan/data/SRR3581866/</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/27549386</t>
+  </si>
+  <si>
+    <t>https://trace.ncbi.nlm.nih.gov/Traces/sra/?run=SRR3581866</t>
+  </si>
+  <si>
+    <t>Flower</t>
+  </si>
+  <si>
+    <t>flower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,6 +303,12 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -400,7 +415,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -421,6 +436,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -772,7 +788,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
@@ -834,8 +850,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S3" totalsRowShown="0">
-  <autoFilter ref="A1:S3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:S4" totalsRowShown="0">
+  <autoFilter ref="A1:S4"/>
   <tableColumns count="19">
     <tableColumn id="1" name="Entry number"/>
     <tableColumn id="10" name="Title*" dataDxfId="17"/>
@@ -1183,35 +1199,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="10.8984375" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.8984375" customWidth="1"/>
-    <col min="6" max="6" width="43.19921875" customWidth="1"/>
-    <col min="7" max="7" width="15.8984375" customWidth="1"/>
-    <col min="8" max="8" width="15.09765625" customWidth="1"/>
-    <col min="9" max="9" width="20.796875" customWidth="1"/>
-    <col min="10" max="10" width="9.8984375" customWidth="1"/>
-    <col min="11" max="11" width="9.09765625" customWidth="1"/>
-    <col min="12" max="12" width="16.3984375" customWidth="1"/>
-    <col min="13" max="13" width="17.59765625" customWidth="1"/>
+    <col min="5" max="5" width="34.875" customWidth="1"/>
+    <col min="6" max="6" width="43.25" customWidth="1"/>
+    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="8" max="8" width="15.125" customWidth="1"/>
+    <col min="9" max="9" width="20.75" customWidth="1"/>
+    <col min="10" max="10" width="9.875" customWidth="1"/>
+    <col min="11" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="16.375" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="20.796875" customWidth="1"/>
-    <col min="17" max="17" width="18.796875" customWidth="1"/>
-    <col min="18" max="18" width="19.3984375" customWidth="1"/>
+    <col min="16" max="16" width="20.75" customWidth="1"/>
+    <col min="17" max="17" width="18.75" customWidth="1"/>
+    <col min="18" max="18" width="19.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1302,7 +1318,7 @@
         <v>41</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>7</v>
@@ -1325,30 +1341,30 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I3" s="10">
         <v>13627154</v>
@@ -1357,26 +1373,71 @@
         <v>41</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="P3" s="10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="12"/>
       <c r="S3" s="12"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="20">
+        <v>25081651</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -1401,20 +1462,20 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.296875" customWidth="1"/>
+    <col min="1" max="2" width="15.25" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="17.296875" customWidth="1"/>
-    <col min="6" max="8" width="20.796875" customWidth="1"/>
+    <col min="5" max="5" width="17.25" customWidth="1"/>
+    <col min="6" max="8" width="20.75" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
     <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="11.296875" customWidth="1"/>
+    <col min="12" max="12" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1439,7 +1500,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1466,45 +1527,45 @@
       <selection activeCell="B8" sqref="B8:T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.296875" customWidth="1"/>
-    <col min="3" max="3" width="10.296875" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="19.19921875" customWidth="1"/>
-    <col min="6" max="6" width="33.59765625" customWidth="1"/>
-    <col min="7" max="7" width="15.19921875" customWidth="1"/>
-    <col min="8" max="8" width="14.8984375" customWidth="1"/>
-    <col min="9" max="9" width="13.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+    <col min="6" max="6" width="33.625" customWidth="1"/>
+    <col min="7" max="7" width="15.25" customWidth="1"/>
+    <col min="8" max="8" width="14.875" customWidth="1"/>
+    <col min="9" max="9" width="13.375" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="21.59765625" customWidth="1"/>
-    <col min="13" max="13" width="14.69921875" customWidth="1"/>
-    <col min="14" max="14" width="18.3984375" customWidth="1"/>
-    <col min="15" max="15" width="18.09765625" customWidth="1"/>
-    <col min="16" max="16" width="17.59765625" customWidth="1"/>
-    <col min="17" max="17" width="18.3984375" customWidth="1"/>
+    <col min="12" max="12" width="21.625" customWidth="1"/>
+    <col min="13" max="13" width="14.75" customWidth="1"/>
+    <col min="14" max="14" width="18.375" customWidth="1"/>
+    <col min="15" max="15" width="18.125" customWidth="1"/>
+    <col min="16" max="16" width="17.625" customWidth="1"/>
+    <col min="17" max="17" width="18.375" customWidth="1"/>
     <col min="18" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="17.8984375" customWidth="1"/>
-    <col min="20" max="20" width="17.69921875" customWidth="1"/>
+    <col min="19" max="19" width="17.875" customWidth="1"/>
+    <col min="20" max="20" width="17.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>25</v>
       </c>
@@ -1524,7 +1585,7 @@
       <c r="L4" s="14"/>
       <c r="M4" s="14"/>
     </row>
-    <row r="5" spans="1:20" s="13" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
@@ -1544,7 +1605,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:20" s="13" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
       <c r="D6" s="19"/>
@@ -1558,7 +1619,7 @@
       <c r="L6" s="18"/>
       <c r="M6" s="16"/>
     </row>
-    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
         <v>1</v>
       </c>
@@ -1672,22 +1733,22 @@
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1711,14 +1772,14 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1738,7 +1799,7 @@
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>495300</xdr:colOff>
                 <xdr:row>5</xdr:row>
-                <xdr:rowOff>15240</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>2</xdr:col>

</xml_diff>

<commit_message>
Fixed how SVG’s appear and removed leaf
Fixed how SVG’s appear and removed leaf as a tissue option

Fixed the following SVG’s and how they appear in index.html: leaf parts,
stamen, stage 1 flower, internode, whole silique, silique stage 1-5 and
6-10, senescent leaf and all the seed stages. Also fixed how the whole
silique appears in Submission_page.html

Removed leaf as a tissue option from Submission_page.html and
bulk_template.xlsx so there is only one leaf option left: full leaf.
</commit_message>
<xml_diff>
--- a/cgi-bin/Submission_page/bulk_template.xlsx
+++ b/cgi-bin/Submission_page/bulk_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2568" windowWidth="19200" windowHeight="11352" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="3024" windowWidth="19200" windowHeight="11352"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="144">
   <si>
     <t>Controls</t>
   </si>
@@ -307,12 +307,6 @@
   </si>
   <si>
     <t>Internode</t>
-  </si>
-  <si>
-    <t>Leaf</t>
-  </si>
-  <si>
-    <t>leaf</t>
   </si>
   <si>
     <t>All leaf parts</t>
@@ -2556,13 +2550,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>466185</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>167641</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2600,13 +2594,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>466185</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2644,13 +2638,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>470999</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2688,13 +2682,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>267</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>45721</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2732,13 +2726,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>2110</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2776,13 +2770,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>472321</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2820,13 +2814,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>472320</xdr:colOff>
-      <xdr:row>104</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2864,13 +2858,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>459353</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2908,13 +2902,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>459352</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2952,13 +2946,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>462905</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2996,13 +2990,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>462905</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3040,13 +3034,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>117</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>153358</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3084,13 +3078,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>452835</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>137161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3128,13 +3122,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>469215</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3172,13 +3166,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>469214</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3216,13 +3210,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>458425</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3260,13 +3254,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>458425</xdr:colOff>
-      <xdr:row>130</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3304,13 +3298,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>33351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3348,13 +3342,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>126</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>135</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>33351</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3392,13 +3386,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>462982</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3436,13 +3430,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>462982</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3480,13 +3474,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>143</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>9826</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3524,13 +3518,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>143</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>139</xdr:row>
       <xdr:rowOff>9826</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3568,13 +3562,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>147</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>449581</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>145038</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3612,13 +3606,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>147</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>142</xdr:row>
       <xdr:rowOff>145038</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3656,13 +3650,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>470709</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3700,13 +3694,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>470709</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>149</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3744,13 +3738,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>151</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>462368</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>155</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3788,13 +3782,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>151</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>462368</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>155</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3832,13 +3826,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>157</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>160</xdr:row>
       <xdr:rowOff>95052</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3876,13 +3870,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>163</xdr:row>
+      <xdr:row>157</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>166</xdr:row>
+      <xdr:row>160</xdr:row>
       <xdr:rowOff>95052</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3920,13 +3914,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>162</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>465656</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3964,13 +3958,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>162</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>465656</xdr:colOff>
-      <xdr:row>170</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4008,13 +4002,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>172</xdr:row>
+      <xdr:row>166</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>168</xdr:row>
       <xdr:rowOff>70045</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4052,13 +4046,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>176</xdr:row>
+      <xdr:row>170</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>178</xdr:row>
+      <xdr:row>172</xdr:row>
       <xdr:rowOff>79309</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4096,13 +4090,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>464230</xdr:colOff>
-      <xdr:row>183</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4140,13 +4134,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>180</xdr:row>
+      <xdr:row>174</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>464230</xdr:colOff>
-      <xdr:row>183</xdr:row>
+      <xdr:row>177</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4184,13 +4178,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>15241</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>179</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>188</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>37011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4228,13 +4222,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>185</xdr:row>
+      <xdr:row>179</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>188</xdr:row>
+      <xdr:row>182</xdr:row>
       <xdr:rowOff>37011</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4272,13 +4266,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>190</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>465003</xdr:colOff>
-      <xdr:row>193</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4316,13 +4310,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>195</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>467010</xdr:colOff>
-      <xdr:row>198</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4360,13 +4354,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>200</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>470781</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>15241</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4404,13 +4398,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>200</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>470780</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4448,13 +4442,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>205</xdr:row>
+      <xdr:row>199</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>207</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>190846</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4492,13 +4486,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>209</xdr:row>
+      <xdr:row>203</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>449581</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>205</xdr:row>
       <xdr:rowOff>147209</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4536,13 +4530,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:row>207</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>209</xdr:row>
       <xdr:rowOff>86361</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4580,13 +4574,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:row>207</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>209</xdr:row>
       <xdr:rowOff>86360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4624,13 +4618,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1089</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4668,13 +4662,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1089</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4712,13 +4706,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>222</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>225</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>45129</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4756,13 +4750,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>227</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>461945</xdr:colOff>
-      <xdr:row>230</xdr:row>
+      <xdr:row>224</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4800,13 +4794,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>232</xdr:row>
+      <xdr:row>226</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>463227</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>228</xdr:row>
       <xdr:rowOff>144781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4844,13 +4838,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>236</xdr:row>
+      <xdr:row>230</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>464821</xdr:colOff>
-      <xdr:row>238</xdr:row>
+      <xdr:row>232</xdr:row>
       <xdr:rowOff>71251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4888,13 +4882,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>236</xdr:row>
+      <xdr:row>230</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>238</xdr:row>
+      <xdr:row>232</xdr:row>
       <xdr:rowOff>71251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4975,8 +4969,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="F1:F29" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="F1:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="F1:F28" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="F1:F28"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Tissues*"/>
   </tableColumns>
@@ -4985,8 +4979,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="H1:H23" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="H1:H23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="H1:H22" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="H1:H22"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Tissues subunit*"/>
   </tableColumns>
@@ -5318,7 +5312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -5441,7 +5435,7 @@
         <v>24</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>5</v>
@@ -5450,7 +5444,7 @@
         <v>6</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
@@ -5520,7 +5514,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -5530,12 +5524,12 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5549,7 +5543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
@@ -5613,7 +5607,7 @@
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -21623,11 +21617,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H237"/>
+  <dimension ref="A1:H231"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <pane ySplit="7" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -21873,144 +21867,144 @@
         <v>75</v>
       </c>
       <c r="G72" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" t="s">
-        <v>78</v>
-      </c>
       <c r="F78" t="s">
         <v>77</v>
       </c>
       <c r="G78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="83" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F83" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F90" t="s">
+        <v>81</v>
+      </c>
+      <c r="G90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" t="s">
+        <v>83</v>
+      </c>
+      <c r="F97" t="s">
+        <v>83</v>
+      </c>
+      <c r="G97" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="84" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F84" t="s">
-        <v>79</v>
-      </c>
-      <c r="G84" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="89" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F89" t="s">
-        <v>81</v>
-      </c>
-      <c r="G89" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="96" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F96" t="s">
-        <v>83</v>
-      </c>
-      <c r="G96" t="s">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B103" t="s">
+      <c r="C101" t="s">
         <v>85</v>
       </c>
-      <c r="C103" t="s">
-        <v>85</v>
-      </c>
-      <c r="F103" t="s">
-        <v>85</v>
-      </c>
-      <c r="G103" t="s">
+      <c r="F101" t="s">
+        <v>84</v>
+      </c>
+      <c r="G101" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B107" t="s">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
         <v>86</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C106" t="s">
         <v>87</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F106" t="s">
         <v>86</v>
       </c>
-      <c r="G107" t="s">
+      <c r="G106" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B112" t="s">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F110" t="s">
+        <v>89</v>
+      </c>
+      <c r="G110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F114" t="s">
         <v>88</v>
       </c>
-      <c r="C112" t="s">
-        <v>89</v>
-      </c>
-      <c r="F112" t="s">
-        <v>88</v>
-      </c>
-      <c r="G112" t="s">
+      <c r="G114" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>91</v>
+      </c>
+      <c r="C118" t="s">
+        <v>90</v>
+      </c>
+      <c r="F118" t="s">
+        <v>91</v>
+      </c>
+      <c r="G118" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F116" t="s">
-        <v>91</v>
-      </c>
-      <c r="G116" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F120" t="s">
-        <v>90</v>
-      </c>
-      <c r="G120" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>92</v>
+      </c>
+      <c r="C122" t="s">
         <v>93</v>
       </c>
-      <c r="C124" t="s">
+      <c r="F122" t="s">
         <v>92</v>
       </c>
-      <c r="F124" t="s">
-        <v>93</v>
-      </c>
-      <c r="G124" t="s">
+      <c r="G122" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
         <v>94</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C127" t="s">
         <v>95</v>
       </c>
-      <c r="F128" t="s">
+      <c r="F127" t="s">
         <v>94</v>
       </c>
-      <c r="G128" t="s">
+      <c r="G127" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B133" t="s">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>97</v>
+      </c>
+      <c r="C132" t="s">
         <v>96</v>
       </c>
-      <c r="C133" t="s">
+      <c r="F132" t="s">
         <v>97</v>
       </c>
-      <c r="F133" t="s">
-        <v>96</v>
-      </c>
-      <c r="G133" t="s">
+      <c r="G132" t="s">
         <v>44</v>
       </c>
     </row>
@@ -22028,45 +22022,45 @@
         <v>44</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B144" t="s">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
         <v>101</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C142" t="s">
         <v>100</v>
       </c>
-      <c r="F144" t="s">
+      <c r="F142" t="s">
         <v>101</v>
       </c>
-      <c r="G144" t="s">
+      <c r="G142" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B148" t="s">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
         <v>103</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C145" t="s">
         <v>102</v>
       </c>
-      <c r="F148" t="s">
+      <c r="F145" t="s">
         <v>103</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G145" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B151" t="s">
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B152" t="s">
         <v>105</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C152" t="s">
         <v>104</v>
       </c>
-      <c r="F151" t="s">
+      <c r="F152" t="s">
         <v>105</v>
       </c>
-      <c r="G151" t="s">
+      <c r="G152" t="s">
         <v>44</v>
       </c>
     </row>
@@ -22084,191 +22078,178 @@
         <v>44</v>
       </c>
     </row>
-    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B164" t="s">
+    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B163" t="s">
         <v>109</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C163" t="s">
         <v>108</v>
       </c>
-      <c r="F164" t="s">
+      <c r="F163" t="s">
         <v>109</v>
       </c>
-      <c r="G164" t="s">
+      <c r="G163" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B169" t="s">
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F167" t="s">
+        <v>110</v>
+      </c>
+      <c r="G167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F171" t="s">
         <v>111</v>
       </c>
-      <c r="C169" t="s">
-        <v>110</v>
-      </c>
-      <c r="F169" t="s">
-        <v>111</v>
-      </c>
-      <c r="G169" t="s">
+      <c r="G171" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>113</v>
+      </c>
+      <c r="C175" t="s">
+        <v>114</v>
+      </c>
+      <c r="F175" t="s">
+        <v>113</v>
+      </c>
+      <c r="G175" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B180" t="s">
+        <v>116</v>
+      </c>
+      <c r="C180" t="s">
+        <v>116</v>
+      </c>
+      <c r="F180" t="s">
+        <v>116</v>
+      </c>
+      <c r="G180" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F173" t="s">
-        <v>112</v>
-      </c>
-      <c r="G173" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F177" t="s">
-        <v>113</v>
-      </c>
-      <c r="G177" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B181" t="s">
-        <v>115</v>
-      </c>
-      <c r="C181" t="s">
-        <v>116</v>
-      </c>
-      <c r="F181" t="s">
-        <v>115</v>
-      </c>
-      <c r="G181" t="s">
+    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F185" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B186" t="s">
+      <c r="G185" t="s">
         <v>118</v>
       </c>
-      <c r="C186" t="s">
-        <v>118</v>
-      </c>
-      <c r="F186" t="s">
-        <v>118</v>
-      </c>
-      <c r="G186" t="s">
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F190" t="s">
+        <v>119</v>
+      </c>
+      <c r="G190" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B195" t="s">
+        <v>122</v>
+      </c>
+      <c r="C195" t="s">
+        <v>121</v>
+      </c>
+      <c r="F195" t="s">
+        <v>122</v>
+      </c>
+      <c r="G195" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F191" t="s">
-        <v>119</v>
-      </c>
-      <c r="G191" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F196" t="s">
-        <v>121</v>
-      </c>
-      <c r="G196" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="201" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B201" t="s">
+    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F200" t="s">
+        <v>123</v>
+      </c>
+      <c r="G200" t="s">
         <v>124</v>
       </c>
-      <c r="C201" t="s">
-        <v>123</v>
-      </c>
-      <c r="F201" t="s">
-        <v>124</v>
-      </c>
-      <c r="G201" t="s">
+    </row>
+    <row r="204" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F204" t="s">
+        <v>126</v>
+      </c>
+      <c r="G204" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="208" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B208" t="s">
+        <v>127</v>
+      </c>
+      <c r="C208" t="s">
+        <v>128</v>
+      </c>
+      <c r="F208" t="s">
+        <v>127</v>
+      </c>
+      <c r="G208" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="206" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F206" t="s">
-        <v>125</v>
-      </c>
-      <c r="G206" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="210" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F210" t="s">
-        <v>128</v>
-      </c>
-      <c r="G210" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="214" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B214" t="s">
+    <row r="212" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B212" t="s">
+        <v>130</v>
+      </c>
+      <c r="C212" t="s">
         <v>129</v>
       </c>
-      <c r="C214" t="s">
+      <c r="F212" t="s">
         <v>130</v>
       </c>
-      <c r="F214" t="s">
-        <v>129</v>
-      </c>
-      <c r="G214" t="s">
+      <c r="G212" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="218" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B218" t="s">
+    <row r="217" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F217" t="s">
+        <v>131</v>
+      </c>
+      <c r="G217" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="222" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F222" t="s">
+        <v>133</v>
+      </c>
+      <c r="G222" t="s">
         <v>132</v>
       </c>
-      <c r="C218" t="s">
-        <v>131</v>
-      </c>
-      <c r="F218" t="s">
-        <v>132</v>
-      </c>
-      <c r="G218" t="s">
+    </row>
+    <row r="227" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="F227" t="s">
+        <v>135</v>
+      </c>
+      <c r="G227" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="231" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B231" t="s">
+        <v>30</v>
+      </c>
+      <c r="C231" t="s">
+        <v>30</v>
+      </c>
+      <c r="F231" t="s">
+        <v>136</v>
+      </c>
+      <c r="G231" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="223" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F223" t="s">
-        <v>133</v>
-      </c>
-      <c r="G223" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="228" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F228" t="s">
-        <v>135</v>
-      </c>
-      <c r="G228" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F233" t="s">
-        <v>137</v>
-      </c>
-      <c r="G233" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="237" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B237" t="s">
-        <v>30</v>
-      </c>
-      <c r="C237" t="s">
-        <v>30</v>
-      </c>
-      <c r="F237" t="s">
-        <v>138</v>
-      </c>
-      <c r="G237" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="k0+RLoOj/hWvm4uAnjJSD9VYVTr+W6UiMch8o9IO+UdjqRWwHWnadUm8xFL7srJKW2Ud4te0G6h9999hwYU2qg==" saltValue="UyNOjPP4ULtjcj/ni5o7Vw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -22282,10 +22263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H29"/>
+  <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -22304,10 +22285,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
@@ -22388,7 +22369,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
         <v>69</v>
@@ -22407,12 +22388,12 @@
         <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H13" t="s">
         <v>80</v>
@@ -22420,7 +22401,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H14" t="s">
         <v>82</v>
@@ -22431,15 +22412,15 @@
         <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
@@ -22447,7 +22428,7 @@
         <v>98</v>
       </c>
       <c r="H17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.3">
@@ -22463,7 +22444,7 @@
         <v>102</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.3">
@@ -22471,7 +22452,7 @@
         <v>104</v>
       </c>
       <c r="H20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.3">
@@ -22479,7 +22460,7 @@
         <v>106</v>
       </c>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.3">
@@ -22492,10 +22473,7 @@
     </row>
     <row r="23" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>110</v>
-      </c>
-      <c r="H23" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="6:8" x14ac:dyDescent="0.3">
@@ -22505,31 +22483,26 @@
     </row>
     <row r="25" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F25" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F26" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F29" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KqJroYiMB2zH7ZGvBOVR3ZHhh3IcjGjsTuJ6GY+SAoRGGapTnf0uxp40JZq4iY1l+4v6rM1LX1bKN8hHr8vU+g==" saltValue="01L+jpbNMpvJT52jpa3C7A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2iOhMu/Zsaetff9xwbqvvxY/aqImueMECJMN6dOOLar8GGIlGyKZxnLJqASJ5M40+cNpGRy8SwidNRGEpKoIYQ==" saltValue="dotnfUMqESzDAbWrlveEIw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">
     <tablePart r:id="rId1"/>

</xml_diff>